<commit_message>
- clean - Data Siliziumtombak
</commit_message>
<xml_diff>
--- a/Visualisierung/Glycerin Wasser gemische 2.xlsx
+++ b/Visualisierung/Glycerin Wasser gemische 2.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25924"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\49151\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\Diss\Software\Hiwi\Visualisierung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1EC6158-0507-4DE8-911A-AAD0D77C4967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{C07BB914-1C87-42C5-901E-CD5AFA350010}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="18240"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,18 +35,27 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={349651E8-9729-454E-90E2-DB2269289F6F}</author>
   </authors>
   <commentList>
-    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{349651E8-9729-454E-90E2-DB2269289F6F}">
+    <comment ref="E5" authorId="0" shapeId="0">
       <text>
-        <t xml:space="preserve">[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     In der zitierten quelle wird ein Linearer Zusammenhang verwendet, da das Molvolumen von Wasser und Glycerin annähernd unabhängig von den Konzentrationen konstant bleibt
 </t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -55,14 +63,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -77,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Isoterm 20 °C</t>
   </si>
@@ -318,12 +326,45 @@
   <si>
     <t>Oberfl.Spannung</t>
   </si>
+  <si>
+    <t>Daten Siliziumtombak:</t>
+  </si>
+  <si>
+    <t>Temp</t>
+  </si>
+  <si>
+    <t>Dichte</t>
+  </si>
+  <si>
+    <t>kinematische Visko.</t>
+  </si>
+  <si>
+    <t>Dynamische Visko.</t>
+  </si>
+  <si>
+    <t>Oberflächenspannung</t>
+  </si>
+  <si>
+    <t>[°C]</t>
+  </si>
+  <si>
+    <t>[kg/m3]</t>
+  </si>
+  <si>
+    <t>[m2/s]</t>
+  </si>
+  <si>
+    <t>[kg/m/s] (= 2 mPa*s)</t>
+  </si>
+  <si>
+    <t>[N/m]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,12 +423,92 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -396,13 +517,23 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Link" xfId="2" builtinId="8"/>
@@ -539,7 +670,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -708,7 +839,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1697188816"/>
@@ -767,7 +898,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1697200464"/>
@@ -784,6 +915,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -791,7 +923,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -815,7 +946,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1430,35 +1561,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E73C5A6D-D71A-47ED-B79D-B50510D6E01C}" name="Tabelle1" displayName="Tabelle1" ref="A5:J16" totalsRowShown="0">
-  <autoFilter ref="A5:J16" xr:uid="{E73C5A6D-D71A-47ED-B79D-B50510D6E01C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A5:J16" totalsRowShown="0">
+  <autoFilter ref="A5:J16"/>
   <tableColumns count="10">
-    <tableColumn id="8" xr3:uid="{4C181618-FCF7-4BE5-85AE-0D420F977026}" name="Massen  % Wasser" dataDxfId="9" dataCellStyle="Prozent"/>
-    <tableColumn id="7" xr3:uid="{81E61AB0-7640-4316-A30B-556698745FAF}" name="Massen % Glycerin" dataDxfId="8" dataCellStyle="Prozent">
+    <tableColumn id="8" name="Massen  % Wasser" dataDxfId="9" dataCellStyle="Prozent"/>
+    <tableColumn id="7" name="Massen % Glycerin" dataDxfId="8" dataCellStyle="Prozent">
       <calculatedColumnFormula>1-Tabelle1[[#This Row],[Massen  % Wasser]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{680D318B-6569-4B5E-BDD6-BFAFF90D2833}" name="mol % Wasser" dataDxfId="7" dataCellStyle="Prozent">
+    <tableColumn id="1" name="mol % Wasser" dataDxfId="7" dataCellStyle="Prozent">
       <calculatedColumnFormula array="1">(Tabelle1[[#This Row],[Massen  % Wasser]]/Tabelle2[Molmasse Wasser])/((Tabelle1[[#This Row],[Massen  % Wasser]]/Tabelle2[Molmasse Wasser])+(Tabelle1[[#This Row],[Massen % Glycerin]]/Tabelle2[Molmasse Glycerin]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{F9464C83-984D-4886-B28A-BA18C4651E19}" name="mol % Glycerin" dataDxfId="6" dataCellStyle="Prozent">
+    <tableColumn id="2" name="mol % Glycerin" dataDxfId="6" dataCellStyle="Prozent">
       <calculatedColumnFormula array="1">(Tabelle1[[#This Row],[Massen % Glycerin]]/Tabelle2[Molmasse Glycerin])/((Tabelle1[[#This Row],[Massen  % Wasser]]/Tabelle2[Molmasse Wasser])+(Tabelle1[[#This Row],[Massen % Glycerin]]/Tabelle2[Molmasse Glycerin]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{2AACC8F2-DE94-4D73-9E7C-9F05F0DA99CD}" name="Dichte [kg/m^3]" dataDxfId="5">
+    <tableColumn id="3" name="Dichte [kg/m^3]" dataDxfId="5">
       <calculatedColumnFormula array="1" xml:space="preserve"> Tabelle2[ρ0kg/m^3 Wasser]*Tabelle1[[#This Row],[Massen  % Wasser]]+Tabelle2[ρ0kg/m^3 Glycerin]*Tabelle1[[#This Row],[Massen % Glycerin]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{2FF64E77-D8C8-4E3F-B11B-3F8A702CB27B}" name="Vol % Wasser" dataDxfId="4" dataCellStyle="Prozent">
+    <tableColumn id="9" name="Vol % Wasser" dataDxfId="4" dataCellStyle="Prozent">
       <calculatedColumnFormula array="1" xml:space="preserve"> (Tabelle1[[#This Row],[Massen  % Wasser]]/Tabelle2[ρ0kg/m^3 Wasser])/((Tabelle1[[#This Row],[Massen  % Wasser]]/Tabelle2[ρ0kg/m^3 Wasser])+(Tabelle1[[#This Row],[Massen % Glycerin]]/Tabelle2[ρ0kg/m^3 Glycerin]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{F183A7B0-407E-4B93-AA51-93B44393867C}" name="Vol % Glycerin" dataDxfId="3" dataCellStyle="Prozent">
+    <tableColumn id="10" name="Vol % Glycerin" dataDxfId="3" dataCellStyle="Prozent">
       <calculatedColumnFormula array="1" xml:space="preserve"> (Tabelle1[[#This Row],[Massen % Glycerin]]/Tabelle2[ρ0kg/m^3 Glycerin])/((Tabelle1[[#This Row],[Massen  % Wasser]]/Tabelle2[ρ0kg/m^3 Wasser])+(Tabelle1[[#This Row],[Massen % Glycerin]]/Tabelle2[ρ0kg/m^3 Glycerin]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{90B24482-7900-465A-8FE3-AC888688D7BB}" name="Dyn. Viskosität η" dataDxfId="2">
+    <tableColumn id="4" name="Dyn. Viskosität η" dataDxfId="2">
       <calculatedColumnFormula array="1">Tabelle2[η0 '[mPa*s'] Wasser]*((1-(Tabelle1[[#This Row],[Vol % Glycerin]]/Tabelle2[Cm]))/(1-(Tabelle2[k0]*Tabelle2[Cm]-1)*(Tabelle1[[#This Row],[Vol % Glycerin]]/Tabelle2[Cm])))^((-2.5*Tabelle2[Cm])/(2-Tabelle2[k0]*Tabelle2[Cm]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{79E677F2-CBC0-4E80-9ABF-4EB342615182}" name="Kin. Viskosität ν" dataDxfId="1">
+    <tableColumn id="5" name="Kin. Viskosität ν" dataDxfId="1">
       <calculatedColumnFormula>Tabelle1[[#This Row],[Dyn. Viskosität η]]/Tabelle1[[#This Row],[Dichte '[kg/m^3']]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0D456137-42E9-4754-8084-7374B58ADA1E}" name="Oberfl.Spannung" dataDxfId="0">
+    <tableColumn id="6" name="Oberfl.Spannung" dataDxfId="0">
       <calculatedColumnFormula array="1">Tabelle1[[#This Row],[Massen  % Wasser]]*Tabelle2[σ0 '[mN/m'] Wasser]+Tabelle1[[#This Row],[Massen % Glycerin]]*Tabelle2[σ0 '[mN/m'] Glycerin]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1467,23 +1598,23 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F918B8A7-A160-46A6-83D4-C4D8CF823EE4}" name="Tabelle2" displayName="Tabelle2" ref="A2:J3" totalsRowShown="0">
-  <autoFilter ref="A2:J3" xr:uid="{F918B8A7-A160-46A6-83D4-C4D8CF823EE4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="A2:J3" totalsRowShown="0">
+  <autoFilter ref="A2:J3"/>
   <tableColumns count="10">
-    <tableColumn id="3" xr3:uid="{2783DBF1-473C-4207-A37B-6792E11C8204}" name="η0 [mPa*s] Wasser">
+    <tableColumn id="3" name="η0 [mPa*s] Wasser">
       <calculatedColumnFormula>1.001</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F17A040C-9957-46A6-831B-8F2C10781D16}" name="ρ0kg/m^3 Wasser"/>
-    <tableColumn id="5" xr3:uid="{BC117699-2323-461D-8EE1-40ABE9FD25EA}" name="σ0 [mN/m] Wasser"/>
-    <tableColumn id="11" xr3:uid="{AFBDAAE7-4EA7-448E-A153-737CB01C63B5}" name="η0 [mPa*s] Glycerin"/>
-    <tableColumn id="12" xr3:uid="{071551C8-5F85-4255-8B73-B01D2287D72C}" name="ρ0kg/m^3 Glycerin"/>
-    <tableColumn id="13" xr3:uid="{72DD8D39-4E93-45B1-89ED-CBB5E35F7204}" name="σ0 [mN/m] Glycerin"/>
-    <tableColumn id="6" xr3:uid="{F0841C04-D4BD-4DC3-B6AE-DDD625C65BBD}" name="Molmasse Wasser"/>
-    <tableColumn id="7" xr3:uid="{7B0E5CC2-0D73-456A-B495-4719FEEEB480}" name="Molmasse Glycerin"/>
-    <tableColumn id="15" xr3:uid="{8DD3AA9A-4E55-4AF8-9CF6-5F44EB593D89}" name="k0">
+    <tableColumn id="4" name="ρ0kg/m^3 Wasser"/>
+    <tableColumn id="5" name="σ0 [mN/m] Wasser"/>
+    <tableColumn id="11" name="η0 [mPa*s] Glycerin"/>
+    <tableColumn id="12" name="ρ0kg/m^3 Glycerin"/>
+    <tableColumn id="13" name="σ0 [mN/m] Glycerin"/>
+    <tableColumn id="6" name="Molmasse Wasser"/>
+    <tableColumn id="7" name="Molmasse Glycerin"/>
+    <tableColumn id="15" name="k0">
       <calculatedColumnFormula>-0.012*(20+273.15)+4.74</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{84A69E98-4B3F-4007-A41E-C80935FB034D}" name="Cm">
+    <tableColumn id="16" name="Cm">
       <calculatedColumnFormula>1.2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1796,30 +1927,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D7D9D5E-A23D-4C8E-8FA7-315DA08F4E63}">
-  <dimension ref="A1:J22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" customWidth="1"/>
-    <col min="10" max="10" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" customWidth="1"/>
-    <col min="12" max="12" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" customWidth="1"/>
+    <col min="6" max="6" width="20.44140625" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" customWidth="1"/>
+    <col min="9" max="9" width="19.88671875" customWidth="1"/>
+    <col min="10" max="10" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" customWidth="1"/>
+    <col min="12" max="12" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1827,7 +1958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16.5">
+    <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1859,7 +1990,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>1.001</f>
         <v>1.0009999999999999</v>
@@ -1894,7 +2025,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1926,7 +2057,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>0</v>
       </c>
@@ -1965,7 +2096,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>0.1</v>
       </c>
@@ -2004,7 +2135,7 @@
         <v>64.873999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>0.2</v>
       </c>
@@ -2043,7 +2174,7 @@
         <v>65.748000000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>0.3</v>
       </c>
@@ -2082,7 +2213,7 @@
         <v>66.622</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>0.4</v>
       </c>
@@ -2121,7 +2252,7 @@
         <v>67.495999999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
@@ -2160,7 +2291,7 @@
         <v>68.37</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>0.6</v>
       </c>
@@ -2199,7 +2330,7 @@
         <v>69.244</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>0.7</v>
       </c>
@@ -2238,7 +2369,7 @@
         <v>70.117999999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>0.8</v>
       </c>
@@ -2277,7 +2408,7 @@
         <v>70.99199999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>0.9</v>
       </c>
@@ -2316,7 +2447,7 @@
         <v>71.865999999999985</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>1</v>
       </c>
@@ -2355,13 +2486,80 @@
         <v>72.739999999999995</v>
       </c>
     </row>
-    <row r="22" spans="3:3">
+    <row r="18" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="G19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="7"/>
+      <c r="I19" s="8"/>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="G20" s="9"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="11"/>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="G21" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="10">
+        <v>920</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C22" s="3"/>
+      <c r="G22" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="10">
+        <v>1000</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="G23" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="12">
+        <f>H24/H22</f>
+        <v>9.9999999999999986E-10</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="G24" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H24" s="12">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G25" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H25" s="14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I25" s="15" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{145787D5-E667-40BD-B40B-6E52F5DD7C59}"/>
+    <hyperlink ref="B1" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -2378,5 +2576,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A526A064-CC7B-4B19-BC0C-73E0C5F4F168}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A526A064-CC7B-4B19-BC0C-73E0C5F4F168}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/DataMashup"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>